<commit_message>
All missing Jars included
</commit_message>
<xml_diff>
--- a/Meritnation/Test Data/testData.xlsx
+++ b/Meritnation/Test Data/testData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="192">
   <si>
     <t>createAccountTest</t>
   </si>
@@ -585,6 +585,15 @@
   </si>
   <si>
     <t>https://www.meritnation.com/blog</t>
+  </si>
+  <si>
+    <t>MobileSiteRegFromGoogleLnk</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/ask-answer/question/what-is-thermodynamics/light/10698759</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/ask-answer/question/apdhit-gandhyash/hindi/11177221</t>
   </si>
 </sst>
 </file>
@@ -809,7 +818,7 @@
   <dimension ref="A1:P65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2659,6 +2668,17 @@
         <v>188</v>
       </c>
     </row>
+    <row r="146" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -2675,6 +2695,8 @@
     <hyperlink ref="C40" r:id="rId10" display="enggqatest+61@meritnation.com"/>
     <hyperlink ref="D40" r:id="rId11" display="enggqatest+34@meritnation.com"/>
     <hyperlink ref="B43" r:id="rId12" display="https://www.meritnation.com/"/>
+    <hyperlink ref="B146" r:id="rId13" display="https://www.meritnation.com/ask-answer/question/what-is-thermodynamics/light/10698759"/>
+    <hyperlink ref="C146" r:id="rId14" display="https://www.meritnation.com/ask-answer/question/apdhit-gandhyash/hindi/11177221"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Junior live class test
</commit_message>
<xml_diff>
--- a/Meritnation/Test Data/testData.xlsx
+++ b/Meritnation/Test Data/testData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="193">
   <si>
     <t>createAccountTest</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>enggqatest+92@meritnation.com</t>
+  </si>
+  <si>
+    <t>enggqatest+4@meritnation.com</t>
   </si>
   <si>
     <t>MyQaTest</t>
@@ -817,8 +820,8 @@
   </sheetPr>
   <dimension ref="A1:P65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -898,45 +901,48 @@
       <c r="O2" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="P2" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -944,1169 +950,1169 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="J5" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G6" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="L6" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
       <c r="B7" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I7" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="0" t="s">
-        <v>44</v>
-      </c>
       <c r="K7" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
       <c r="B10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
       <c r="B11" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H11" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="K11" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="0" t="s">
+      <c r="L11" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="K11" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="L11" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="M11" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4"/>
       <c r="B12" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F12" s="3"/>
       <c r="H12" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
       <c r="B13" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F13" s="3"/>
       <c r="H13" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F14" s="3"/>
       <c r="J14" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4"/>
       <c r="B16" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="J16" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K16" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="L16" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="M16" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="N16" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="O16" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="L16" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="M16" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="N16" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="O16" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
       <c r="B17" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D17" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="J17" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="K17" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="L17" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="G17" s="0" t="s">
+      <c r="M17" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N17" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="H17" s="0" t="s">
+      <c r="O17" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="M17" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="N17" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="O17" s="0" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
       <c r="B18" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="J18" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="K18" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="L18" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="L18" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="M18" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="N18" s="0" t="s">
-        <v>67</v>
-      </c>
       <c r="O18" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
       <c r="B19" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="M19" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="M19" s="0" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
       <c r="B20" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D20" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>71</v>
-      </c>
       <c r="J20" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4"/>
       <c r="B21" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D21" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="I21" s="0" t="s">
         <v>75</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
       <c r="B23" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D23" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="J23" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="K23" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="L23" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="J23" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="L23" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="M23" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O23" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
       <c r="B24" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
       <c r="B25" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="E25" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
       <c r="B27" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O27" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
       <c r="B28" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O28" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
       <c r="B29" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O29" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
       <c r="B30" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O30" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
       <c r="B31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="O31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
       <c r="B32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
       <c r="B33" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M33" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N33" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="O33" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
       <c r="B34" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M34" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N34" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="O34" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M35" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N35" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="O35" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M36" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N36" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="O36" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="P36" s="8"/>
     </row>
@@ -2129,24 +2135,24 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>13</v>
@@ -2154,529 +2160,529 @@
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2691,12 +2697,13 @@
     <hyperlink ref="M2" r:id="rId6" display="enggqatest+62@meritnation.com"/>
     <hyperlink ref="N2" r:id="rId7" display="enggqatest+93@meritnation.com"/>
     <hyperlink ref="O2" r:id="rId8" display="enggqatest+92@meritnation.com"/>
-    <hyperlink ref="B40" r:id="rId9" display="enggqatest+83@meritnation.com"/>
-    <hyperlink ref="C40" r:id="rId10" display="enggqatest+61@meritnation.com"/>
-    <hyperlink ref="D40" r:id="rId11" display="enggqatest+34@meritnation.com"/>
-    <hyperlink ref="B43" r:id="rId12" display="https://www.meritnation.com/"/>
-    <hyperlink ref="B146" r:id="rId13" display="https://www.meritnation.com/ask-answer/question/what-is-thermodynamics/light/10698759"/>
-    <hyperlink ref="C146" r:id="rId14" display="https://www.meritnation.com/ask-answer/question/apdhit-gandhyash/hindi/11177221"/>
+    <hyperlink ref="P2" r:id="rId9" display="enggqatest+4@meritnation.com"/>
+    <hyperlink ref="B40" r:id="rId10" display="enggqatest+83@meritnation.com"/>
+    <hyperlink ref="C40" r:id="rId11" display="enggqatest+61@meritnation.com"/>
+    <hyperlink ref="D40" r:id="rId12" display="enggqatest+34@meritnation.com"/>
+    <hyperlink ref="B43" r:id="rId13" display="https://www.meritnation.com/"/>
+    <hyperlink ref="B146" r:id="rId14" display="https://www.meritnation.com/ask-answer/question/what-is-thermodynamics/light/10698759"/>
+    <hyperlink ref="C146" r:id="rId15" display="https://www.meritnation.com/ask-answer/question/apdhit-gandhyash/hindi/11177221"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
script for Change the grade and verify header menu added
</commit_message>
<xml_diff>
--- a/Meritnation/Test Data/testData.xlsx
+++ b/Meritnation/Test Data/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="195">
   <si>
     <t>createAccountTest</t>
   </si>
@@ -597,6 +597,12 @@
   </si>
   <si>
     <t>https://www.meritnation.com/ask-answer/question/apdhit-gandhyash/hindi/11177221</t>
+  </si>
+  <si>
+    <t>12thGradePurchaseLinkFromDashboard</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/demo/cbse12-science</t>
   </si>
 </sst>
 </file>
@@ -820,7 +826,7 @@
   </sheetPr>
   <dimension ref="A1:P65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
     </sheetView>
   </sheetViews>
@@ -2720,10 +2726,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2731,6 +2737,14 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.66801619433198"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2755,6 +2769,9 @@
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" display="https://www.meritnation.com/demo/cbse12-science"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added new script for dashboard page
</commit_message>
<xml_diff>
--- a/Meritnation/Test Data/testData.xlsx
+++ b/Meritnation/Test Data/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="197">
   <si>
     <t>createAccountTest</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>enggqatest+4@meritnation.com</t>
+  </si>
+  <si>
+    <t>enggqatest+8@meritnation.com</t>
+  </si>
+  <si>
+    <t>enggqamnchattest@meritnation.com</t>
   </si>
   <si>
     <t>MyQaTest</t>
@@ -824,10 +830,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P65536"/>
+  <dimension ref="A1:R65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -910,45 +916,51 @@
       <c r="P2" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="Q2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -956,1169 +968,1169 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="J5" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="L6" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
       <c r="B7" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="H9" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
       <c r="B10" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
       <c r="B11" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4"/>
       <c r="B12" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F12" s="3"/>
       <c r="H12" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F13" s="3"/>
       <c r="H13" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F14" s="3"/>
       <c r="J14" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4"/>
       <c r="B16" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M16" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="N16" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="N16" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="O16" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
       <c r="B17" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M17" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="N17" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="N17" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="O17" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
       <c r="B18" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="M18" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L18" s="0" t="s">
+      <c r="N18" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="M18" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="N18" s="0" t="s">
-        <v>68</v>
-      </c>
       <c r="O18" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
       <c r="B19" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D19" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="M19" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="M19" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
       <c r="B20" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4"/>
       <c r="B21" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G21" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
       <c r="B23" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="O23" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
       <c r="B24" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>78</v>
-      </c>
       <c r="E24" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
       <c r="B25" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
       <c r="B27" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O27" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
       <c r="B28" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="O28" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
       <c r="B29" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O29" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
       <c r="B30" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="O30" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
       <c r="B31" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="M31" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="N31" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="O31" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
       <c r="B32" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="M32" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="N32" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="O32" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
       <c r="B33" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="M33" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="N33" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="O33" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
       <c r="B34" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="M34" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="N34" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="O34" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="M35" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="N35" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="O35" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="M36" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="N36" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="O36" s="7" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P36" s="8"/>
     </row>
@@ -2141,24 +2153,24 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>13</v>
@@ -2166,529 +2178,529 @@
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2704,12 +2716,13 @@
     <hyperlink ref="N2" r:id="rId7" display="enggqatest+93@meritnation.com"/>
     <hyperlink ref="O2" r:id="rId8" display="enggqatest+92@meritnation.com"/>
     <hyperlink ref="P2" r:id="rId9" display="enggqatest+4@meritnation.com"/>
-    <hyperlink ref="B40" r:id="rId10" display="enggqatest+83@meritnation.com"/>
-    <hyperlink ref="C40" r:id="rId11" display="enggqatest+61@meritnation.com"/>
-    <hyperlink ref="D40" r:id="rId12" display="enggqatest+34@meritnation.com"/>
-    <hyperlink ref="B43" r:id="rId13" display="https://www.meritnation.com/"/>
-    <hyperlink ref="B146" r:id="rId14" display="https://www.meritnation.com/ask-answer/question/what-is-thermodynamics/light/10698759"/>
-    <hyperlink ref="C146" r:id="rId15" display="https://www.meritnation.com/ask-answer/question/apdhit-gandhyash/hindi/11177221"/>
+    <hyperlink ref="Q2" r:id="rId10" display="enggqatest+8@meritnation.com"/>
+    <hyperlink ref="B40" r:id="rId11" display="enggqatest+83@meritnation.com"/>
+    <hyperlink ref="C40" r:id="rId12" display="enggqatest+61@meritnation.com"/>
+    <hyperlink ref="D40" r:id="rId13" display="enggqatest+34@meritnation.com"/>
+    <hyperlink ref="B43" r:id="rId14" display="https://www.meritnation.com/"/>
+    <hyperlink ref="B146" r:id="rId15" display="https://www.meritnation.com/ask-answer/question/what-is-thermodynamics/light/10698759"/>
+    <hyperlink ref="C146" r:id="rId16" display="https://www.meritnation.com/ask-answer/question/apdhit-gandhyash/hindi/11177221"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2728,7 +2741,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2739,10 +2752,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Added new script for Dashboard
</commit_message>
<xml_diff>
--- a/Meritnation/Test Data/testData.xlsx
+++ b/Meritnation/Test Data/testData.xlsx
@@ -833,7 +833,7 @@
   <dimension ref="A1:R65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
+      <selection pane="topLeft" activeCell="Q4" activeCellId="0" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2717,12 +2717,13 @@
     <hyperlink ref="O2" r:id="rId8" display="enggqatest+92@meritnation.com"/>
     <hyperlink ref="P2" r:id="rId9" display="enggqatest+4@meritnation.com"/>
     <hyperlink ref="Q2" r:id="rId10" display="enggqatest+8@meritnation.com"/>
-    <hyperlink ref="B40" r:id="rId11" display="enggqatest+83@meritnation.com"/>
-    <hyperlink ref="C40" r:id="rId12" display="enggqatest+61@meritnation.com"/>
-    <hyperlink ref="D40" r:id="rId13" display="enggqatest+34@meritnation.com"/>
-    <hyperlink ref="B43" r:id="rId14" display="https://www.meritnation.com/"/>
-    <hyperlink ref="B146" r:id="rId15" display="https://www.meritnation.com/ask-answer/question/what-is-thermodynamics/light/10698759"/>
-    <hyperlink ref="C146" r:id="rId16" display="https://www.meritnation.com/ask-answer/question/apdhit-gandhyash/hindi/11177221"/>
+    <hyperlink ref="R2" r:id="rId11" display="enggqamnchattest@meritnation.com"/>
+    <hyperlink ref="B40" r:id="rId12" display="enggqatest+83@meritnation.com"/>
+    <hyperlink ref="C40" r:id="rId13" display="enggqatest+61@meritnation.com"/>
+    <hyperlink ref="D40" r:id="rId14" display="enggqatest+34@meritnation.com"/>
+    <hyperlink ref="B43" r:id="rId15" display="https://www.meritnation.com/"/>
+    <hyperlink ref="B146" r:id="rId16" display="https://www.meritnation.com/ask-answer/question/what-is-thermodynamics/light/10698759"/>
+    <hyperlink ref="C146" r:id="rId17" display="https://www.meritnation.com/ask-answer/question/apdhit-gandhyash/hindi/11177221"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Test Data for tracking api added
</commit_message>
<xml_diff>
--- a/Meritnation/Test Data/testData.xlsx
+++ b/Meritnation/Test Data/testData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="208">
   <si>
     <t>createAccountTest</t>
   </si>
@@ -603,6 +603,39 @@
   </si>
   <si>
     <t>https://www.meritnation.com/ask-answer/question/apdhit-gandhyash/hindi/11177221</t>
+  </si>
+  <si>
+    <t>TrackingAPITest:otypes</t>
+  </si>
+  <si>
+    <t>USER_LOGIN</t>
+  </si>
+  <si>
+    <t>STUDY_LESSON</t>
+  </si>
+  <si>
+    <t>TEST_QUESTION</t>
+  </si>
+  <si>
+    <t>PRACTICE_QUESTION</t>
+  </si>
+  <si>
+    <t>TG_QUESTION_ATTEMPT</t>
+  </si>
+  <si>
+    <t>TEST_GENERATOR</t>
+  </si>
+  <si>
+    <t>VIEW_NCERT_SOLUTION</t>
+  </si>
+  <si>
+    <t>ORDER_CREATE</t>
+  </si>
+  <si>
+    <t>VIEW_QUESTION</t>
+  </si>
+  <si>
+    <t>ASK_QUESTION</t>
   </si>
   <si>
     <t>12thGradePurchaseLinkFromDashboard</t>
@@ -832,8 +865,8 @@
   </sheetPr>
   <dimension ref="A1:R65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q4" activeCellId="0" sqref="Q4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B157" activeCellId="0" sqref="B157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2701,6 +2734,59 @@
       </c>
       <c r="C146" s="2" t="s">
         <v>194</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B147" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B148" s="0" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B149" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B150" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B151" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B152" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B153" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B154" s="0" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B155" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B156" s="0" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2753,10 +2839,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>